<commit_message>
Allow cleaned CSV in .gitignore, add cleaned data
</commit_message>
<xml_diff>
--- a/expense_log_day2.xlsx
+++ b/expense_log_day2.xlsx
@@ -2,29 +2,41 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\Data-Portfolio\expense_log_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data Analytics\Data-Portfolio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4559C81F-7366-455C-B795-D77599117C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ECF369-9296-4667-9D66-A3E475FD881C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pivot_Category" sheetId="5" r:id="rId1"/>
     <sheet name="Day1" sheetId="1" r:id="rId2"/>
     <sheet name="Monthly Net-Cashflow" sheetId="4" r:id="rId3"/>
+    <sheet name="Dashboard_Day3" sheetId="6" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Day1'!$A$1:$E$16</definedName>
+    <definedName name="Slicer_Category">#N/A</definedName>
+    <definedName name="Slicer_Category1">#N/A</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="31" r:id="rId4"/>
+    <pivotCache cacheId="0" r:id="rId5"/>
   </pivotCaches>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
+      <x14:slicerCaches>
+        <x14:slicerCache r:id="rId6"/>
+        <x14:slicerCache r:id="rId7"/>
+      </x14:slicerCaches>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -41,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="40">
   <si>
     <t>Date</t>
   </si>
@@ -159,6 +171,9 @@
   <si>
     <t>Column Labels</t>
   </si>
+  <si>
+    <t>Personal Spending Dashboard (june 2025 Dummy Data)</t>
+  </si>
 </sst>
 </file>
 
@@ -167,9 +182,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="m/d/yyyy"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="167" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="166" formatCode="d/m/yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -203,8 +218,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -215,6 +237,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFD9D9D9"/>
         <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -258,7 +286,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -289,14 +317,17 @@
       <alignment horizontal="left" indent="1"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="5">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -314,11 +345,6 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FFFF0000"/>
       </font>
       <fill>
@@ -327,6 +353,21 @@
           <bgColor rgb="FFB7E1CD"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -724,7 +765,7 @@
           </c:val>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-7855-4A26-A829-0C664F79B545}"/>
+              <c16:uniqueId val="{00000001-0FB4-4C93-A264-86A0626BE655}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -947,7 +988,1203 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[expense_log_day2.xlsx]Dashboard_Day3!PivotTable1</c:name>
+    <c:fmtId val="20"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-AU"/>
+              <a:t>Spending by Category</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+      <c:pivotFmt>
+        <c:idx val="1"/>
+        <c:spPr>
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dashboard_Day3!$B$2:$B$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2025-06</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dashboard_Day3!$A$4:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Dining</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Entertainment</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fuel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Gift</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Groceries</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Internet</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Rent</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Salary</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Utilities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dashboard_Day3!$B$4:$B$13</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-18.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-205.89999999999998</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-318</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-79.989999999999995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-1900</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3850</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-180.6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3EA1-4029-8859-BE6921312EE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dashboard_Day3!$C$2:$C$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>2025-07</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Dashboard_Day3!$A$4:$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>Dining</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Entertainment</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Fuel</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Gift</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Groceries</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Internet</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Rent</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>Salary</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>Utilities</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dashboard_Day3!$C$4:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>"$"#,##0.00</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-18.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-40</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-50</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-65.3</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3850</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3EA1-4029-8859-BE6921312EE6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1085849504"/>
+        <c:axId val="1085850944"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1085849504"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1085850944"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1085850944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="&quot;$&quot;#,##0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1085849504"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:pivotSource>
+    <c:name>[expense_log_day2.xlsx]Dashboard_Day3!PivotTable3</c:name>
+    <c:fmtId val="7"/>
+  </c:pivotSource>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Net Cash-flow</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> by Month</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:pivotFmts>
+      <c:pivotFmt>
+        <c:idx val="0"/>
+        <c:spPr>
+          <a:ln w="28575" cap="rnd">
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:marker>
+          <c:symbol val="none"/>
+        </c:marker>
+        <c:dLbl>
+          <c:idx val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:spAutoFit/>
+            </a:bodyPr>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="75000"/>
+                      <a:lumOff val="25000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
+          </c:extLst>
+        </c:dLbl>
+      </c:pivotFmt>
+    </c:pivotFmts>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Dashboard_Day3!$B$15</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:multiLvlStrRef>
+              <c:f>Dashboard_Day3!$A$16:$A$33</c:f>
+              <c:multiLvlStrCache>
+                <c:ptCount val="15"/>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>Dining</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>Entertainment</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Fuel</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Gift</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Groceries</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Internet</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Rent</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Salary</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Utilities</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Dining</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Entertainment</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Fuel</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Gift</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Groceries</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Salary</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="0">
+                    <c:v>2025-06</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>2025-07</c:v>
+                  </c:pt>
+                </c:lvl>
+              </c:multiLvlStrCache>
+            </c:multiLvlStrRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Dashboard_Day3!$B$16:$B$33</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>-3.9168277506187532E-3</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-5.2930104738091255E-3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-4.3593234262291954E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-1.0586020947618251E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-6.7327093226852083E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-1.6935516311999677E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.40226879600949356</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.81512361296660529</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>-3.8236707662797124E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>-3.9168277506187532E-3</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>-5.2930104738091255E-3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>-8.4688167580946015E-3</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>-1.0586020947618251E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>-1.3825343357589436E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.81512361296660529</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E8D2-48E0-969F-848C7C847F30}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1196013328"/>
+        <c:axId val="1196012848"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1196013328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1196012848"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1196012848"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1196013328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+  <c:extLst>
+    <c:ext xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" uri="{781A3756-C4B2-4CAC-9D66-4F8BD8637D16}">
+      <c14:pivotOptions>
+        <c14:dropZoneFilter val="1"/>
+        <c14:dropZoneCategories val="1"/>
+        <c14:dropZoneData val="1"/>
+        <c14:dropZoneSeries val="1"/>
+        <c14:dropZonesVisible val="1"/>
+      </c14:pivotOptions>
+    </c:ext>
+    <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{E28EC0CA-F0BB-4C9C-879D-F8772B89E7AC}">
+      <c16:pivotOptions16>
+        <c16:showExpandCollapseFieldButtons val="1"/>
+      </c16:pivotOptions16>
+    </c:ext>
+  </c:extLst>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1492,19 +2729,1038 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>106680</xdr:colOff>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>3810</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>167640</xdr:colOff>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>64770</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1530,6 +3786,473 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>15240</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Category">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B44906B2-2EF5-D295-A979-72E8D2022EF4}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Category"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="3933825" y="333375"/>
+              <a:ext cx="2095500" cy="2724150"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>350520</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Category 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B4B62D55-CC41-F865-04F6-A1B8D5C29B5B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Category 1"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="2867025" y="371475"/>
+              <a:ext cx="2295525" cy="2619375"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Category 2">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4590CDE5-D67A-4143-942B-C7FCB4069B99}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Category 2"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5457825" y="219075"/>
+              <a:ext cx="2095500" cy="2724150"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="3" name="Category 3">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8108A9F1-DF6B-4272-8030-C031E55EA65C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2010/slicer">
+              <sle:slicer xmlns:sle="http://schemas.microsoft.com/office/drawing/2010/slicer" name="Category 3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="5486400" y="3152775"/>
+              <a:ext cx="2305050" cy="2619375"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-AU" sz="1100"/>
+                <a:t>This shape represents a slicer. Slicers are supported in Excel 2010 or later.
+If the shape was modified in an earlier version of Excel, or if the workbook was saved in Excel 2003 or earlier, the slicer cannot be used.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>87630</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>213360</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>148590</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{40B479FD-A0C3-A530-D306-D3A3C6576680}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>184784</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>99059</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>59054</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>163829</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2010007F-0561-BFA7-0FFC-40778FB908A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>533400</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F99EA612-193E-76F0-886F-0362FD6B36F6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="533400" y="6391275"/>
+          <a:ext cx="5572125" cy="514350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:shade val="50000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-AU" sz="1100" i="1"/>
+            <a:t>Use the slicers on the right to filter this dashboard dynamically by Category or Month.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-AU" sz="1100" i="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1539,7 +4262,7 @@
     <worksheetSource ref="A1:F23" sheet="Day1"/>
   </cacheSource>
   <cacheFields count="6">
-    <cacheField name="Date" numFmtId="167">
+    <cacheField name="Date" numFmtId="166">
       <sharedItems containsSemiMixedTypes="0" containsNonDate="0" containsDate="1" containsString="0" minDate="2025-06-16T00:00:00" maxDate="2025-07-27T00:00:00"/>
     </cacheField>
     <cacheField name="Category" numFmtId="0">
@@ -1573,7 +4296,7 @@
   </cacheFields>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition/>
+      <x14:pivotCacheDefinition pivotCacheId="1912680444"/>
     </ext>
   </extLst>
 </pivotCacheDefinition>
@@ -1761,10 +4484,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF85E118-DED0-4860-9B4A-ACF7CB7966AD}" name="PivotTable4" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{CF85E118-DED0-4860-9B4A-ACF7CB7966AD}" name="PivotTable4" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="19">
   <location ref="A3:D14" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="6">
-    <pivotField numFmtId="167" showAll="0"/>
+    <pivotField numFmtId="166" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="10">
         <item x="1"/>
@@ -1843,7 +4566,7 @@
     <dataField name="Sum of Amount (NZD)" fld="3" baseField="0" baseItem="0" numFmtId="165"/>
   </dataFields>
   <conditionalFormats count="2">
-    <conditionalFormat priority="2">
+    <conditionalFormat priority="1">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -1869,7 +4592,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="1">
+    <conditionalFormat priority="2">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="3">
@@ -1935,10 +4658,10 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CB5545A-88EE-43AD-9FA2-FCE05A7E53C3}" name="PivotTable3" cacheId="31" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5CB5545A-88EE-43AD-9FA2-FCE05A7E53C3}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="6">
-    <pivotField numFmtId="167" showAll="0"/>
+    <pivotField numFmtId="166" showAll="0"/>
     <pivotField axis="axisRow" showAll="0">
       <items count="10">
         <item x="1"/>
@@ -2040,6 +4763,390 @@
     </ext>
   </extLst>
 </pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00A6507B-EABB-4963-99AE-E990EF780077}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="8">
+  <location ref="A15:B33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField numFmtId="166" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="10">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="5"/>
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="18">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Amount (NZD)" fld="3" showDataAs="percentOfTotal" baseField="0" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <chartFormats count="1">
+    <chartFormat chart="7" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="1">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{94547B55-F111-4A9F-A185-65F4AE08FE67}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="21">
+  <location ref="A2:D13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField numFmtId="166" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="10">
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="8"/>
+        <item x="0"/>
+        <item x="7"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" numFmtId="165" showAll="0"/>
+    <pivotField numFmtId="165" showAll="0"/>
+    <pivotField axis="axisCol" showAll="0">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="10">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="5"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Amount (NZD)" fld="3" baseField="0" baseItem="0" numFmtId="165"/>
+  </dataFields>
+  <conditionalFormats count="2">
+    <conditionalFormat priority="1">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="9">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+            </reference>
+            <reference field="5" count="2" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+    <conditionalFormat priority="2">
+      <pivotAreas count="1">
+        <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
+          <references count="3">
+            <reference field="4294967294" count="1" selected="0">
+              <x v="0"/>
+            </reference>
+            <reference field="1" count="9">
+              <x v="0"/>
+              <x v="1"/>
+              <x v="2"/>
+              <x v="3"/>
+              <x v="4"/>
+              <x v="5"/>
+              <x v="6"/>
+              <x v="7"/>
+              <x v="8"/>
+            </reference>
+            <reference field="5" count="2" selected="0">
+              <x v="0"/>
+              <x v="1"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotAreas>
+    </conditionalFormat>
+  </conditionalFormats>
+  <chartFormats count="4">
+    <chartFormat chart="18" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="18" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="20" format="0" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+    <chartFormat chart="20" format="1" series="1">
+      <pivotArea type="data" outline="0" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="0"/>
+          </reference>
+          <reference field="5" count="1" selected="0">
+            <x v="1"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </chartFormat>
+  </chartFormats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Category" xr10:uid="{1E2DD343-9E5A-4A15-81FE-03FE09ABF17E}" sourceName="Category">
+  <pivotTables>
+    <pivotTable tabId="5" name="PivotTable4"/>
+    <pivotTable tabId="6" name="PivotTable1"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1912680444">
+      <items count="9">
+        <i x="1" s="1"/>
+        <i x="2" s="1"/>
+        <i x="3" s="1"/>
+        <i x="4" s="1"/>
+        <i x="5" s="1"/>
+        <i x="6" s="1"/>
+        <i x="8" s="1"/>
+        <i x="0" s="1"/>
+        <i x="7" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicerCaches/slicerCache2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10" name="Slicer_Category1" xr10:uid="{76BC152C-314B-4BFA-AF47-A66C0AB10AD8}" sourceName="Category">
+  <pivotTables>
+    <pivotTable tabId="4" name="PivotTable3"/>
+    <pivotTable tabId="6" name="PivotTable3"/>
+  </pivotTables>
+  <data>
+    <tabular pivotCacheId="1912680444">
+      <items count="9">
+        <i x="1" s="1"/>
+        <i x="2" s="1"/>
+        <i x="3" s="1"/>
+        <i x="4" s="1"/>
+        <i x="5" s="1"/>
+        <i x="6" s="1"/>
+        <i x="8" s="1"/>
+        <i x="0" s="1"/>
+        <i x="7" s="1"/>
+      </items>
+    </tabular>
+  </data>
+</slicerCacheDefinition>
+</file>
+
+<file path=xl/slicers/slicer1.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Category" xr10:uid="{BA46E6E5-937D-44D1-AF91-A9732C94CED2}" cache="Slicer_Category" caption="Category" rowHeight="209550"/>
+</slicers>
+</file>
+
+<file path=xl/slicers/slicer2.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Category 1" xr10:uid="{6790AD84-8D81-46B8-AD01-C163A6267BE8}" cache="Slicer_Category1" caption="Category" rowHeight="209550"/>
+</slicers>
+</file>
+
+<file path=xl/slicers/slicer3.xml><?xml version="1.0" encoding="utf-8"?>
+<slicers xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x xr10">
+  <slicer name="Category 2" xr10:uid="{A6F05B49-508D-4F1E-A73C-95C95E068D2A}" cache="Slicer_Category" caption="Category" rowHeight="209550"/>
+  <slicer name="Category 3" xr10:uid="{92F6BF01-9813-4738-9CC3-E4E5B3B335B9}" cache="Slicer_Category1" caption="Category" rowHeight="209550"/>
+</slicers>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2242,8 +5349,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05B8C794-8047-4285-931B-C750473CA709}">
   <dimension ref="A3:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:C13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -2412,17 +5519,24 @@
     </row>
   </sheetData>
   <conditionalFormatting pivot="1" sqref="B5:C13">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting pivot="1" sqref="B5:C13">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -6926,7 +10040,7 @@
   </sheetData>
   <autoFilter ref="A1:E16" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <conditionalFormatting sqref="D1:D1007">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6939,7 +10053,7 @@
   <dimension ref="A3:B21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A3" sqref="A3:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -7110,5 +10224,380 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId3"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953BEA47-379D-49CC-8721-00EF5B050D65}">
+  <dimension ref="A1:M33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="N38" sqref="N38"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A1" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="15">
+        <v>-18.5</v>
+      </c>
+      <c r="C4" s="15">
+        <v>-18.5</v>
+      </c>
+      <c r="D4" s="15">
+        <v>-37</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="15">
+        <v>-25</v>
+      </c>
+      <c r="C5" s="15">
+        <v>-25</v>
+      </c>
+      <c r="D5" s="15">
+        <v>-50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="15">
+        <v>-205.89999999999998</v>
+      </c>
+      <c r="C6" s="15">
+        <v>-40</v>
+      </c>
+      <c r="D6" s="15">
+        <v>-245.89999999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="15">
+        <v>-50</v>
+      </c>
+      <c r="C7" s="15">
+        <v>-50</v>
+      </c>
+      <c r="D7" s="15">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" s="15">
+        <v>-318</v>
+      </c>
+      <c r="C8" s="15">
+        <v>-65.3</v>
+      </c>
+      <c r="D8" s="15">
+        <v>-383.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="15">
+        <v>-79.989999999999995</v>
+      </c>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15">
+        <v>-79.989999999999995</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="15">
+        <v>-1900</v>
+      </c>
+      <c r="C10" s="15"/>
+      <c r="D10" s="15">
+        <v>-1900</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="15">
+        <v>3850</v>
+      </c>
+      <c r="C11" s="15">
+        <v>3850</v>
+      </c>
+      <c r="D11" s="15">
+        <v>7700</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="15">
+        <v>-180.6</v>
+      </c>
+      <c r="C12" s="15"/>
+      <c r="D12" s="15">
+        <v>-180.6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" s="15">
+        <v>1072.0100000000002</v>
+      </c>
+      <c r="C13" s="15">
+        <v>3651.2</v>
+      </c>
+      <c r="D13" s="15">
+        <v>4723.2099999999991</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" s="17">
+        <v>0.22696640632112489</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="17">
+        <v>-3.9168277506187532E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="17">
+        <v>-5.2930104738091255E-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" s="17">
+        <v>-4.3593234262291954E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="17">
+        <v>-1.0586020947618251E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B21" s="17">
+        <v>-6.7327093226852083E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" s="17">
+        <v>-1.6935516311999677E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23" s="17">
+        <v>-0.40226879600949356</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B24" s="17">
+        <v>0.81512361296660529</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="16" t="s">
+        <v>24</v>
+      </c>
+      <c r="B25" s="17">
+        <v>-3.8236707662797124E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="17">
+        <v>0.77303359367887514</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" s="17">
+        <v>-3.9168277506187532E-3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="17">
+        <v>-5.2930104738091255E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B29" s="17">
+        <v>-8.4688167580946015E-3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B30" s="17">
+        <v>-1.0586020947618251E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="B31" s="17">
+        <v>-1.3825343357589436E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="17">
+        <v>0.81512361296660529</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="B33" s="17">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:M1"/>
+  </mergeCells>
+  <conditionalFormatting pivot="1" sqref="B4:C12">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="B4:C12">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
+      <x14:slicerList>
+        <x14:slicer r:id="rId4"/>
+      </x14:slicerList>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>